<commit_message>
check for server talk
</commit_message>
<xml_diff>
--- a/app/dummy.xlsx
+++ b/app/dummy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7510739665e2ad5/Sandbox/Full App/base-app/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{BBE60B36-E530-4F19-96FE-AE75E4D9A477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7FF319E-ECE7-4531-8F66-50D0457964F5}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{BBE60B36-E530-4F19-96FE-AE75E4D9A477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32A3FB45-93AF-41AB-A7AD-797FA4A92934}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B2BD2526-8C16-43A5-8328-F40CCEB79115}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{B2BD2526-8C16-43A5-8328-F40CCEB79115}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calibrate" sheetId="1" r:id="rId1"/>
+    <sheet name="Policy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -53,15 +54,48 @@
   <si>
     <t>Policy 1</t>
   </si>
+  <si>
+    <t>Unemployement</t>
+  </si>
+  <si>
+    <t>Policy Implemented</t>
+  </si>
+  <si>
+    <t>Param 1</t>
+  </si>
+  <si>
+    <t>Param 2</t>
+  </si>
+  <si>
+    <t>Param 3</t>
+  </si>
+  <si>
+    <t>Param 4</t>
+  </si>
+  <si>
+    <t>Policy 4</t>
+  </si>
+  <si>
+    <t>Policy 5</t>
+  </si>
+  <si>
+    <t>Policy 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -404,19 +438,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A573565E-5135-4146-AABF-1BDC667510E0}">
-  <dimension ref="A1:G398"/>
+  <dimension ref="A1:F398"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12.3125" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,86 +466,83 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>43891</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>43892</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>43893</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>43894</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>43895</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>43896</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>43897</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>43898</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>43899</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>43900</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>43901</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>43902</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>43903</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>43904</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>43905</v>
       </c>
@@ -2428,4 +2461,2087 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1C956E-065B-4963-BA34-381BA1B74519}">
+  <dimension ref="A1:S399"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>43892</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
+        <v>43893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
+        <v>43894</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
+        <v>43895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <v>43896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
+        <v>43897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <v>43898</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1">
+        <v>43908</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1">
+        <v>43910</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1">
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1">
+        <v>43918</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1">
+        <v>43919</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1">
+        <v>43925</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1">
+        <v>43926</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1">
+        <v>43928</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1">
+        <v>43929</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1">
+        <v>43930</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1">
+        <v>43932</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1">
+        <v>43933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1">
+        <v>43935</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1">
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1">
+        <v>43939</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1">
+        <v>43944</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1">
+        <v>43946</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1">
+        <v>43947</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1">
+        <v>43948</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1">
+        <v>43949</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="1">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1">
+        <v>43955</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="1">
+        <v>43959</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1">
+        <v>43961</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1">
+        <v>43962</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1">
+        <v>43963</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1">
+        <v>43967</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="1">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1">
+        <v>43969</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1">
+        <v>43970</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1">
+        <v>43972</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1">
+        <v>43974</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1">
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1">
+        <v>43981</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1">
+        <v>43982</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1">
+        <v>43984</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1">
+        <v>43988</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="1">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="1">
+        <v>43991</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="1">
+        <v>43992</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="1">
+        <v>43993</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="1">
+        <v>43994</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="1">
+        <v>43995</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="1">
+        <v>43996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="1">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="1">
+        <v>43998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="1">
+        <v>43999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="1">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="1">
+        <v>44001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="1">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="1">
+        <v>44003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="1">
+        <v>44004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="1">
+        <v>44005</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="1">
+        <v>44006</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="1">
+        <v>44007</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="1">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="1">
+        <v>44009</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="1">
+        <v>44010</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="1">
+        <v>44011</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="1">
+        <v>44014</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1">
+        <v>44016</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1">
+        <v>44017</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="1">
+        <v>44018</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="1">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="1">
+        <v>44020</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="1">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="1">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="1">
+        <v>44023</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="1">
+        <v>44024</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="1">
+        <v>44025</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="1">
+        <v>44026</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="1">
+        <v>44027</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="1">
+        <v>44028</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="1">
+        <v>44029</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="1">
+        <v>44030</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="1">
+        <v>44031</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="1">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="1">
+        <v>44033</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="1">
+        <v>44034</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="1">
+        <v>44035</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="1">
+        <v>44036</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="1">
+        <v>44037</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="1">
+        <v>44038</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="1">
+        <v>44039</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="1">
+        <v>44040</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="1">
+        <v>44041</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="1">
+        <v>44042</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="1">
+        <v>44043</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="1">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="1">
+        <v>44045</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="1">
+        <v>44046</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="1">
+        <v>44047</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="1">
+        <v>44048</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="1">
+        <v>44049</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="1">
+        <v>44050</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="1">
+        <v>44051</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="1">
+        <v>44052</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="1">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="1">
+        <v>44054</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="1">
+        <v>44056</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="1">
+        <v>44057</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="1">
+        <v>44058</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="1">
+        <v>44059</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="1">
+        <v>44060</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="1">
+        <v>44061</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="1">
+        <v>44062</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="1">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="1">
+        <v>44064</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="1">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="1">
+        <v>44066</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="1">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="1">
+        <v>44068</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="1">
+        <v>44069</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="1">
+        <v>44070</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="1">
+        <v>44071</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="1">
+        <v>44072</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="1">
+        <v>44073</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="1">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="1">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="1">
+        <v>44076</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="1">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="1">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="1">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="1">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="1">
+        <v>44081</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="1">
+        <v>44082</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="1">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="1">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="1">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="1">
+        <v>44086</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="1">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="1">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="1">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" s="1">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="1">
+        <v>44092</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="1">
+        <v>44093</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" s="1">
+        <v>44094</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="1">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="1">
+        <v>44096</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="1">
+        <v>44097</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="1">
+        <v>44098</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="1">
+        <v>44099</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" s="1">
+        <v>44100</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" s="1">
+        <v>44101</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" s="1">
+        <v>44102</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" s="1">
+        <v>44103</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" s="1">
+        <v>44104</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" s="1">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" s="1">
+        <v>44106</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" s="1">
+        <v>44107</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" s="1">
+        <v>44108</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="1">
+        <v>44109</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" s="1">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223" s="1">
+        <v>44111</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" s="1">
+        <v>44112</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" s="1">
+        <v>44113</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" s="1">
+        <v>44114</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" s="1">
+        <v>44115</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228" s="1">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229" s="1">
+        <v>44117</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A230" s="1">
+        <v>44118</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A231" s="1">
+        <v>44119</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A232" s="1">
+        <v>44120</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A233" s="1">
+        <v>44121</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A234" s="1">
+        <v>44122</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A235" s="1">
+        <v>44123</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A236" s="1">
+        <v>44124</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237" s="1">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238" s="1">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239" s="1">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A240" s="1">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241" s="1">
+        <v>44129</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242" s="1">
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A243" s="1">
+        <v>44131</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244" s="1">
+        <v>44132</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A245" s="1">
+        <v>44133</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A246" s="1">
+        <v>44134</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A247" s="1">
+        <v>44135</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248" s="1">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="1">
+        <v>44137</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="1">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251" s="1">
+        <v>44139</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="1">
+        <v>44140</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253" s="1">
+        <v>44141</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="1">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255" s="1">
+        <v>44143</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256" s="1">
+        <v>44144</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257" s="1">
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258" s="1">
+        <v>44146</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A259" s="1">
+        <v>44147</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A260" s="1">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261" s="1">
+        <v>44149</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A262" s="1">
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A263" s="1">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A264" s="1">
+        <v>44152</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A265" s="1">
+        <v>44153</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A266" s="1">
+        <v>44154</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A267" s="1">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A268" s="1">
+        <v>44156</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A269" s="1">
+        <v>44157</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A270" s="1">
+        <v>44158</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A271" s="1">
+        <v>44159</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A272" s="1">
+        <v>44160</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A273" s="1">
+        <v>44161</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A274" s="1">
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A275" s="1">
+        <v>44163</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A276" s="1">
+        <v>44164</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A277" s="1">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A278" s="1">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A279" s="1">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A280" s="1">
+        <v>44168</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A281" s="1">
+        <v>44169</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A282" s="1">
+        <v>44170</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A283" s="1">
+        <v>44171</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A284" s="1">
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A285" s="1">
+        <v>44173</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A286" s="1">
+        <v>44174</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A287" s="1">
+        <v>44175</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A288" s="1">
+        <v>44176</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A289" s="1">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A290" s="1">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A291" s="1">
+        <v>44179</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A292" s="1">
+        <v>44180</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A293" s="1">
+        <v>44181</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A294" s="1">
+        <v>44182</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A295" s="1">
+        <v>44183</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A296" s="1">
+        <v>44184</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A297" s="1">
+        <v>44185</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A298" s="1">
+        <v>44186</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A299" s="1">
+        <v>44187</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A300" s="1">
+        <v>44188</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A301" s="1">
+        <v>44189</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A302" s="1">
+        <v>44190</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A303" s="1">
+        <v>44191</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A304" s="1">
+        <v>44192</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A305" s="1">
+        <v>44193</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A306" s="1">
+        <v>44194</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A307" s="1">
+        <v>44195</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A308" s="1">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A309" s="1">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A310" s="1">
+        <v>44198</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A311" s="1">
+        <v>44199</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A312" s="1">
+        <v>44200</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A313" s="1">
+        <v>44201</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A314" s="1">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A315" s="1">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A316" s="1">
+        <v>44204</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A317" s="1">
+        <v>44205</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A318" s="1">
+        <v>44206</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A319" s="1">
+        <v>44207</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A320" s="1">
+        <v>44208</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A321" s="1">
+        <v>44209</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A322" s="1">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A323" s="1">
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A324" s="1">
+        <v>44212</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A325" s="1">
+        <v>44213</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A326" s="1">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A327" s="1">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A328" s="1">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A329" s="1">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A330" s="1">
+        <v>44218</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A331" s="1">
+        <v>44219</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A332" s="1">
+        <v>44220</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A333" s="1">
+        <v>44221</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A334" s="1">
+        <v>44222</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A335" s="1">
+        <v>44223</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A336" s="1">
+        <v>44224</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A337" s="1">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A338" s="1">
+        <v>44226</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A339" s="1">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A340" s="1">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A341" s="1">
+        <v>44229</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A342" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A343" s="1">
+        <v>44231</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A344" s="1">
+        <v>44232</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A345" s="1">
+        <v>44233</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A346" s="1">
+        <v>44234</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A347" s="1">
+        <v>44235</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A348" s="1">
+        <v>44236</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A349" s="1">
+        <v>44237</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A350" s="1">
+        <v>44238</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A351" s="1">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A352" s="1">
+        <v>44240</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A353" s="1">
+        <v>44241</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A354" s="1">
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A355" s="1">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A356" s="1">
+        <v>44244</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A357" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A358" s="1">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A359" s="1">
+        <v>44247</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A360" s="1">
+        <v>44248</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A361" s="1">
+        <v>44249</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A362" s="1">
+        <v>44250</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A363" s="1">
+        <v>44251</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A364" s="1">
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A365" s="1">
+        <v>44253</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A366" s="1">
+        <v>44254</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A367" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A368" s="1">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A369" s="1">
+        <v>44257</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A370" s="1">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A371" s="1">
+        <v>44259</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A372" s="1">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A373" s="1">
+        <v>44261</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A374" s="1">
+        <v>44262</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A375" s="1">
+        <v>44263</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A376" s="1">
+        <v>44264</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A377" s="1">
+        <v>44265</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A378" s="1">
+        <v>44266</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A379" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A380" s="1">
+        <v>44268</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A381" s="1">
+        <v>44269</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A382" s="1">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A383" s="1">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A384" s="1">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A385" s="1">
+        <v>44273</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A386" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A387" s="1">
+        <v>44275</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A388" s="1">
+        <v>44276</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A389" s="1">
+        <v>44277</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A390" s="1">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A391" s="1">
+        <v>44279</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A392" s="1">
+        <v>44280</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A393" s="1">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A394" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A395" s="1">
+        <v>44283</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A396" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A397" s="1">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A398" s="1">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A399" s="1">
+        <v>44287</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>